<commit_message>
Add Figure 2 and Figure 3 R codes
</commit_message>
<xml_diff>
--- a/simulation_results_lognormal.xlsx
+++ b/simulation_results_lognormal.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gokcedeliorman/Desktop/PHD/Second_paper_misspesification_lognormal_and_tdist/log_normal_sim_result_excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gokcedeliorman/Documents/GitHub/misspecification_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6ADC9D-A16C-E44A-9CDF-F516F5F7C797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD8D643-1CF6-F140-9627-625D62EF6696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16840" xr2:uid="{8AD9E622-D7DB-524A-A2FB-07D30BA90834}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="first_data" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="590">
   <si>
     <t>ICA_normal</t>
   </si>
@@ -981,6 +982,831 @@
   </si>
   <si>
     <t>0.02274311</t>
+  </si>
+  <si>
+    <t>0.200689</t>
+  </si>
+  <si>
+    <t>0.03268849</t>
+  </si>
+  <si>
+    <t>0.1807996</t>
+  </si>
+  <si>
+    <t>0.5995742</t>
+  </si>
+  <si>
+    <t>0.2280632</t>
+  </si>
+  <si>
+    <t>-0.4775597</t>
+  </si>
+  <si>
+    <t>0.2488576</t>
+  </si>
+  <si>
+    <t>0.1090815</t>
+  </si>
+  <si>
+    <t>-0.3302748</t>
+  </si>
+  <si>
+    <t>0.3930163</t>
+  </si>
+  <si>
+    <t>0.3629198</t>
+  </si>
+  <si>
+    <t>-0.6024283</t>
+  </si>
+  <si>
+    <t>0.1054904</t>
+  </si>
+  <si>
+    <t>0.005757907</t>
+  </si>
+  <si>
+    <t>-0.07588088</t>
+  </si>
+  <si>
+    <t>0.2088076</t>
+  </si>
+  <si>
+    <t>0.1194798</t>
+  </si>
+  <si>
+    <t>0.3456586</t>
+  </si>
+  <si>
+    <t>0.2886493</t>
+  </si>
+  <si>
+    <t>0.09761966</t>
+  </si>
+  <si>
+    <t>-0.3124414</t>
+  </si>
+  <si>
+    <t>0.4287994</t>
+  </si>
+  <si>
+    <t>0.00159005</t>
+  </si>
+  <si>
+    <t>0.03987544</t>
+  </si>
+  <si>
+    <t>0.2167481</t>
+  </si>
+  <si>
+    <t>0.05373969</t>
+  </si>
+  <si>
+    <t>-0.2318182</t>
+  </si>
+  <si>
+    <t>0.04506012</t>
+  </si>
+  <si>
+    <t>0.01086501</t>
+  </si>
+  <si>
+    <t>0.1042354</t>
+  </si>
+  <si>
+    <t>0.5390827</t>
+  </si>
+  <si>
+    <t>0.4748615</t>
+  </si>
+  <si>
+    <t>0.6891019</t>
+  </si>
+  <si>
+    <t>0.1095808</t>
+  </si>
+  <si>
+    <t>0.04057234</t>
+  </si>
+  <si>
+    <t>0.2014258</t>
+  </si>
+  <si>
+    <t>0.3327651</t>
+  </si>
+  <si>
+    <t>0.1272964</t>
+  </si>
+  <si>
+    <t>-0.3567862</t>
+  </si>
+  <si>
+    <t>0.1282084</t>
+  </si>
+  <si>
+    <t>0.01828477</t>
+  </si>
+  <si>
+    <t>-0.1352212</t>
+  </si>
+  <si>
+    <t>0.07440895</t>
+  </si>
+  <si>
+    <t>0.0008566887</t>
+  </si>
+  <si>
+    <t>0.02926925</t>
+  </si>
+  <si>
+    <t>0.1431336</t>
+  </si>
+  <si>
+    <t>0.03825925</t>
+  </si>
+  <si>
+    <t>0.1955997</t>
+  </si>
+  <si>
+    <t>0.3505639</t>
+  </si>
+  <si>
+    <t>0.2677745</t>
+  </si>
+  <si>
+    <t>-0.5174693</t>
+  </si>
+  <si>
+    <t>0.3128992</t>
+  </si>
+  <si>
+    <t>0.09993448</t>
+  </si>
+  <si>
+    <t>-0.3161242</t>
+  </si>
+  <si>
+    <t>0.2032857</t>
+  </si>
+  <si>
+    <t>0.1751481</t>
+  </si>
+  <si>
+    <t>-0.4185069</t>
+  </si>
+  <si>
+    <t>0.1466142</t>
+  </si>
+  <si>
+    <t>0.04796915</t>
+  </si>
+  <si>
+    <t>0.2190186</t>
+  </si>
+  <si>
+    <t>0.07245672</t>
+  </si>
+  <si>
+    <t>0.01266071</t>
+  </si>
+  <si>
+    <t>0.1125198</t>
+  </si>
+  <si>
+    <t>0.04222979</t>
+  </si>
+  <si>
+    <t>0.01903178</t>
+  </si>
+  <si>
+    <t>-0.1379557</t>
+  </si>
+  <si>
+    <t>0.3937361</t>
+  </si>
+  <si>
+    <t>0.1468197</t>
+  </si>
+  <si>
+    <t>-0.3831706</t>
+  </si>
+  <si>
+    <t>0.5728044</t>
+  </si>
+  <si>
+    <t>0.3168317</t>
+  </si>
+  <si>
+    <t>-0.562878</t>
+  </si>
+  <si>
+    <t>0.07481789</t>
+  </si>
+  <si>
+    <t>0.002120229</t>
+  </si>
+  <si>
+    <t>0.04604594</t>
+  </si>
+  <si>
+    <t>0.2326734</t>
+  </si>
+  <si>
+    <t>0.160873</t>
+  </si>
+  <si>
+    <t>0.4010898</t>
+  </si>
+  <si>
+    <t>0.2852666</t>
+  </si>
+  <si>
+    <t>0.1981778</t>
+  </si>
+  <si>
+    <t>0.4451717</t>
+  </si>
+  <si>
+    <t>0.2498088</t>
+  </si>
+  <si>
+    <t>0.0009233291</t>
+  </si>
+  <si>
+    <t>0.03038633</t>
+  </si>
+  <si>
+    <t>0.1201551</t>
+  </si>
+  <si>
+    <t>0.01415725</t>
+  </si>
+  <si>
+    <t>0.1189842</t>
+  </si>
+  <si>
+    <t>0.1717436</t>
+  </si>
+  <si>
+    <t>0.02979049</t>
+  </si>
+  <si>
+    <t>0.1725992</t>
+  </si>
+  <si>
+    <t>0.1361709</t>
+  </si>
+  <si>
+    <t>0.03298342</t>
+  </si>
+  <si>
+    <t>0.1816134</t>
+  </si>
+  <si>
+    <t>0.2463725</t>
+  </si>
+  <si>
+    <t>0.1526736</t>
+  </si>
+  <si>
+    <t>-0.3907346</t>
+  </si>
+  <si>
+    <t>0.01953392</t>
+  </si>
+  <si>
+    <t>0.001992707</t>
+  </si>
+  <si>
+    <t>-0.04463975</t>
+  </si>
+  <si>
+    <t>0.4641822</t>
+  </si>
+  <si>
+    <t>0.1754675</t>
+  </si>
+  <si>
+    <t>-0.4188884</t>
+  </si>
+  <si>
+    <t>0.1543745</t>
+  </si>
+  <si>
+    <t>0.106433</t>
+  </si>
+  <si>
+    <t>0.3262407</t>
+  </si>
+  <si>
+    <t>0.3353994</t>
+  </si>
+  <si>
+    <t>0.2725403</t>
+  </si>
+  <si>
+    <t>-0.5220539</t>
+  </si>
+  <si>
+    <t>0.5845196</t>
+  </si>
+  <si>
+    <t>0.4480102</t>
+  </si>
+  <si>
+    <t>-0.6693357</t>
+  </si>
+  <si>
+    <t>0.06279441</t>
+  </si>
+  <si>
+    <t>0.0007141365</t>
+  </si>
+  <si>
+    <t>0.02672333</t>
+  </si>
+  <si>
+    <t>0.1050975</t>
+  </si>
+  <si>
+    <t>0.001315714</t>
+  </si>
+  <si>
+    <t>0.03627278</t>
+  </si>
+  <si>
+    <t>0.1768835</t>
+  </si>
+  <si>
+    <t>0.09486643</t>
+  </si>
+  <si>
+    <t>-0.3080039</t>
+  </si>
+  <si>
+    <t>0.4513817</t>
+  </si>
+  <si>
+    <t>0.3101728</t>
+  </si>
+  <si>
+    <t>-0.5569316</t>
+  </si>
+  <si>
+    <t>0.2569968</t>
+  </si>
+  <si>
+    <t>0.1368756</t>
+  </si>
+  <si>
+    <t>-0.3699671</t>
+  </si>
+  <si>
+    <t>0.478085</t>
+  </si>
+  <si>
+    <t>0.270554</t>
+  </si>
+  <si>
+    <t>-0.5201481</t>
+  </si>
+  <si>
+    <t>0.05598912</t>
+  </si>
+  <si>
+    <t>0.01432111</t>
+  </si>
+  <si>
+    <t>0.1196708</t>
+  </si>
+  <si>
+    <t>0.07633528</t>
+  </si>
+  <si>
+    <t>0.006647895</t>
+  </si>
+  <si>
+    <t>-0.08153463</t>
+  </si>
+  <si>
+    <t>0.1570277</t>
+  </si>
+  <si>
+    <t>0.004388874</t>
+  </si>
+  <si>
+    <t>-0.06624858</t>
+  </si>
+  <si>
+    <t>0.08132389</t>
+  </si>
+  <si>
+    <t>0.03047564</t>
+  </si>
+  <si>
+    <t>0.1745727</t>
+  </si>
+  <si>
+    <t>0.1843647</t>
+  </si>
+  <si>
+    <t>0.007084343</t>
+  </si>
+  <si>
+    <t>-0.08416854</t>
+  </si>
+  <si>
+    <t>0.2492751</t>
+  </si>
+  <si>
+    <t>0.1106794</t>
+  </si>
+  <si>
+    <t>-0.3326851</t>
+  </si>
+  <si>
+    <t>0.2346809</t>
+  </si>
+  <si>
+    <t>0.0604116</t>
+  </si>
+  <si>
+    <t>-0.2457877</t>
+  </si>
+  <si>
+    <t>0.2232264</t>
+  </si>
+  <si>
+    <t>0.04529462</t>
+  </si>
+  <si>
+    <t>0.2128253</t>
+  </si>
+  <si>
+    <t>0.3164941</t>
+  </si>
+  <si>
+    <t>0.058068</t>
+  </si>
+  <si>
+    <t>-0.240973</t>
+  </si>
+  <si>
+    <t>0.4108584</t>
+  </si>
+  <si>
+    <t>0.04186976</t>
+  </si>
+  <si>
+    <t>0.204621</t>
+  </si>
+  <si>
+    <t>0.2180927</t>
+  </si>
+  <si>
+    <t>0.1542105</t>
+  </si>
+  <si>
+    <t>0.3926965</t>
+  </si>
+  <si>
+    <t>0.2142605</t>
+  </si>
+  <si>
+    <t>0.157802</t>
+  </si>
+  <si>
+    <t>-0.397243</t>
+  </si>
+  <si>
+    <t>0.09817667</t>
+  </si>
+  <si>
+    <t>0.02435137</t>
+  </si>
+  <si>
+    <t>0.1560493</t>
+  </si>
+  <si>
+    <t>0.1629501</t>
+  </si>
+  <si>
+    <t>0.001077225</t>
+  </si>
+  <si>
+    <t>-0.0328211</t>
+  </si>
+  <si>
+    <t>0.1039471</t>
+  </si>
+  <si>
+    <t>0.001934554</t>
+  </si>
+  <si>
+    <t>-0.04398357</t>
+  </si>
+  <si>
+    <t>0.07497166</t>
+  </si>
+  <si>
+    <t>0.05268657</t>
+  </si>
+  <si>
+    <t>0.2295355</t>
+  </si>
+  <si>
+    <t>0.1330247</t>
+  </si>
+  <si>
+    <t>0.03871753</t>
+  </si>
+  <si>
+    <t>-0.1967677</t>
+  </si>
+  <si>
+    <t>0.1176557</t>
+  </si>
+  <si>
+    <t>0.02032874</t>
+  </si>
+  <si>
+    <t>0.1425789</t>
+  </si>
+  <si>
+    <t>0.1518912</t>
+  </si>
+  <si>
+    <t>0.004711212</t>
+  </si>
+  <si>
+    <t>-0.06863827</t>
+  </si>
+  <si>
+    <t>0.126527</t>
+  </si>
+  <si>
+    <t>0.08274154</t>
+  </si>
+  <si>
+    <t>-0.2876483</t>
+  </si>
+  <si>
+    <t>0.221766</t>
+  </si>
+  <si>
+    <t>0.1488973</t>
+  </si>
+  <si>
+    <t>-0.3858721</t>
+  </si>
+  <si>
+    <t>0.5316989</t>
+  </si>
+  <si>
+    <t>0.1499439</t>
+  </si>
+  <si>
+    <t>-0.387226</t>
+  </si>
+  <si>
+    <t>0.1549431</t>
+  </si>
+  <si>
+    <t>0.04671377</t>
+  </si>
+  <si>
+    <t>0.2161337</t>
+  </si>
+  <si>
+    <t>0.1050281</t>
+  </si>
+  <si>
+    <t>0.008173098</t>
+  </si>
+  <si>
+    <t>-0.09040519</t>
+  </si>
+  <si>
+    <t>0.3676915</t>
+  </si>
+  <si>
+    <t>0.1912377</t>
+  </si>
+  <si>
+    <t>-0.4373073</t>
+  </si>
+  <si>
+    <t>0.1610801</t>
+  </si>
+  <si>
+    <t>0.01992584</t>
+  </si>
+  <si>
+    <t>0.1411589</t>
+  </si>
+  <si>
+    <t>0.07081583</t>
+  </si>
+  <si>
+    <t>0.01707515</t>
+  </si>
+  <si>
+    <t>-0.1306719</t>
+  </si>
+  <si>
+    <t>0.0523504</t>
+  </si>
+  <si>
+    <t>0.0292784</t>
+  </si>
+  <si>
+    <t>0.1711093</t>
+  </si>
+  <si>
+    <t>0.2818186</t>
+  </si>
+  <si>
+    <t>0.1120401</t>
+  </si>
+  <si>
+    <t>-0.3347238</t>
+  </si>
+  <si>
+    <t>0.08544584</t>
+  </si>
+  <si>
+    <t>0.0003013958</t>
+  </si>
+  <si>
+    <t>-0.01736075</t>
+  </si>
+  <si>
+    <t>0.3272737</t>
+  </si>
+  <si>
+    <t>0.1236104</t>
+  </si>
+  <si>
+    <t>-0.3515828</t>
+  </si>
+  <si>
+    <t>0.05903823</t>
+  </si>
+  <si>
+    <t>0.0141235</t>
+  </si>
+  <si>
+    <t>0.1188423</t>
+  </si>
+  <si>
+    <t>0.4847342</t>
+  </si>
+  <si>
+    <t>0.1187427</t>
+  </si>
+  <si>
+    <t>-0.3445906</t>
+  </si>
+  <si>
+    <t>0.1510911</t>
+  </si>
+  <si>
+    <t>0.05647878</t>
+  </si>
+  <si>
+    <t>-0.2376526</t>
+  </si>
+  <si>
+    <t>0.1269692</t>
+  </si>
+  <si>
+    <t>0.01535286</t>
+  </si>
+  <si>
+    <t>-0.1239067</t>
+  </si>
+  <si>
+    <t>0.2654774</t>
+  </si>
+  <si>
+    <t>0.2069163</t>
+  </si>
+  <si>
+    <t>-0.4548805</t>
+  </si>
+  <si>
+    <t>0.04724031</t>
+  </si>
+  <si>
+    <t>0.02332465</t>
+  </si>
+  <si>
+    <t>0.1527241</t>
+  </si>
+  <si>
+    <t>0.3962399</t>
+  </si>
+  <si>
+    <t>0.1540094</t>
+  </si>
+  <si>
+    <t>-0.3924403</t>
+  </si>
+  <si>
+    <t>0.3834339</t>
+  </si>
+  <si>
+    <t>0.06477545</t>
+  </si>
+  <si>
+    <t>-0.2545102</t>
+  </si>
+  <si>
+    <t>0.1059553</t>
+  </si>
+  <si>
+    <t>0.00186969</t>
+  </si>
+  <si>
+    <t>-0.04323991</t>
+  </si>
+  <si>
+    <t>0.0847783</t>
+  </si>
+  <si>
+    <t>-0.0001230459</t>
+  </si>
+  <si>
+    <t>0.03156125</t>
+  </si>
+  <si>
+    <t>0.01862716</t>
+  </si>
+  <si>
+    <t>0.1364814</t>
+  </si>
+  <si>
+    <t>0.09244055</t>
+  </si>
+  <si>
+    <t>0.03270614</t>
+  </si>
+  <si>
+    <t>-0.1808484</t>
+  </si>
+  <si>
+    <t>0.04820809</t>
+  </si>
+  <si>
+    <t>0.02992925</t>
+  </si>
+  <si>
+    <t>0.1730007</t>
+  </si>
+  <si>
+    <t>0.3482859</t>
+  </si>
+  <si>
+    <t>0.17594</t>
+  </si>
+  <si>
+    <t>-0.419452</t>
+  </si>
+  <si>
+    <t>0.1989616</t>
+  </si>
+  <si>
+    <t>0.04011705</t>
+  </si>
+  <si>
+    <t>-0.2002924</t>
+  </si>
+  <si>
+    <t>0.27786</t>
+  </si>
+  <si>
+    <t>0.05790541</t>
+  </si>
+  <si>
+    <t>-0.2406354</t>
+  </si>
+  <si>
+    <t>0.1373233</t>
+  </si>
+  <si>
+    <t>0.002579708</t>
+  </si>
+  <si>
+    <t>0.05079083</t>
+  </si>
+  <si>
+    <t>0.1749459</t>
+  </si>
+  <si>
+    <t>0.04284291</t>
+  </si>
+  <si>
+    <t>-0.2069853</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1856,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1347,10 +2179,1185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9896FE6-3DF3-2A4E-8CBF-1B6E66764375}">
+  <dimension ref="A1:C105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>336</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>339</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>342</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>345</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C12" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>351</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="C14" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>354</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C15" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>357</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C16" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>360</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C17" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>363</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C18" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>366</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C19" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>369</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C20" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>372</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="C21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>375</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="C22" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>378</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C23" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>381</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C24" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>384</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="C25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>387</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="C26" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>390</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C27" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>393</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C28" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>396</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="C29" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>399</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="C30" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>402</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C31" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>405</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C32" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>408</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="C33" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>411</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C34" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>414</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C35" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>417</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="C36" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>420</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C37" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>423</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="C38" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>426</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="C39" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>429</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C40" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>432</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="C41" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>435</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="C42" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>438</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C43" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>441</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C44" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>444</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="C45" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>447</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="C46" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>450</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C47" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>453</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="C48" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>456</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="C49" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>459</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C50" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>462</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="C51" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>465</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="C52" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>468</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="C53" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>471</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C54" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>474</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="C55" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>477</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C56" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>480</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="C57" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>483</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="C58" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>486</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="C59" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>489</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="C60" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>492</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C61" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>495</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="C62" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>498</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="C63" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>501</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="C64" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>504</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="C65" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>507</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="C66" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>510</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="C67" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>513</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="C68" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>516</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="C69" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>519</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="C70" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>522</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="C71" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>525</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="C72" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>528</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="C73" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>531</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="C74" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>534</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="C75" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>537</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="C76" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>540</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="C77" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>543</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="C78" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>546</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="C79" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>549</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="C80" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>552</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="C81" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>555</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="C82" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>558</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="C83" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>561</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="C84" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>564</v>
+      </c>
+      <c r="B85" s="4">
+        <v>1.51403E-3</v>
+      </c>
+      <c r="C85" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>566</v>
+      </c>
+      <c r="B86" t="s">
+        <v>567</v>
+      </c>
+      <c r="C86" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>569</v>
+      </c>
+      <c r="B87" t="s">
+        <v>570</v>
+      </c>
+      <c r="C87" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>572</v>
+      </c>
+      <c r="B88" t="s">
+        <v>573</v>
+      </c>
+      <c r="C88" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>575</v>
+      </c>
+      <c r="B89" t="s">
+        <v>576</v>
+      </c>
+      <c r="C89" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>578</v>
+      </c>
+      <c r="B90" t="s">
+        <v>579</v>
+      </c>
+      <c r="C90" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>581</v>
+      </c>
+      <c r="B91" t="s">
+        <v>582</v>
+      </c>
+      <c r="C91" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>584</v>
+      </c>
+      <c r="B92" t="s">
+        <v>585</v>
+      </c>
+      <c r="C92" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>587</v>
+      </c>
+      <c r="B93" t="s">
+        <v>588</v>
+      </c>
+      <c r="C93" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>280</v>
+      </c>
+      <c r="B94" t="s">
+        <v>281</v>
+      </c>
+      <c r="C94" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>283</v>
+      </c>
+      <c r="B95" t="s">
+        <v>284</v>
+      </c>
+      <c r="C95" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>286</v>
+      </c>
+      <c r="B96" t="s">
+        <v>287</v>
+      </c>
+      <c r="C96" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>289</v>
+      </c>
+      <c r="B97" t="s">
+        <v>290</v>
+      </c>
+      <c r="C97" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>292</v>
+      </c>
+      <c r="B98" t="s">
+        <v>293</v>
+      </c>
+      <c r="C98" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>295</v>
+      </c>
+      <c r="B99" t="s">
+        <v>296</v>
+      </c>
+      <c r="C99" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>298</v>
+      </c>
+      <c r="B100" t="s">
+        <v>299</v>
+      </c>
+      <c r="C100" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>301</v>
+      </c>
+      <c r="B101" t="s">
+        <v>302</v>
+      </c>
+      <c r="C101" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>304</v>
+      </c>
+      <c r="B102" t="s">
+        <v>305</v>
+      </c>
+      <c r="C102" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>307</v>
+      </c>
+      <c r="B103" t="s">
+        <v>308</v>
+      </c>
+      <c r="C103" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>310</v>
+      </c>
+      <c r="B104" t="s">
+        <v>311</v>
+      </c>
+      <c r="C104" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>280</v>
+      </c>
+      <c r="B105" t="s">
+        <v>281</v>
+      </c>
+      <c r="C105" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE9C029-B65D-944E-8F0A-8ED4E6E7A9ED}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A87" zoomScale="125" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>